<commit_message>
adicionando exemplos de turmas na planilha matriculas
</commit_message>
<xml_diff>
--- a/matriculas.xlsx
+++ b/matriculas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lrepo\Documents\V4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5129E606-9A33-4EBE-BE49-F1F4F74CAE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA16951-4533-4B0C-A099-561950FA1622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3AA4CDC3-9F67-4144-BE60-7726C1EB9A09}"/>
   </bookViews>
@@ -35,10 +35,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>segqua1112</t>
+  </si>
+  <si>
+    <t>terqui0910</t>
+  </si>
+  <si>
+    <t>segqua2122</t>
+  </si>
+  <si>
+    <t>terqui1314</t>
+  </si>
+  <si>
+    <t>segqua0708</t>
+  </si>
+  <si>
+    <t>terqui1415</t>
+  </si>
+  <si>
+    <t>manel, bernardo, pipico</t>
+  </si>
+  <si>
+    <t>ana, alice, andré</t>
+  </si>
+  <si>
+    <t>thales, amanda, letícia</t>
+  </si>
+  <si>
+    <t>natasha, luisa, gabriela</t>
+  </si>
+  <si>
+    <t>mariana, davi, eduardo</t>
+  </si>
+  <si>
+    <t>rafael, jennifer, luiz</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -66,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +452,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225AD2C9-7D17-4033-8D02-E4EFB3767F2D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>